<commit_message>
big update these jenny
aggiunto tutto (spero) quello che mancava
</commit_message>
<xml_diff>
--- a/jenny_CMF/data/radio.xlsx
+++ b/jenny_CMF/data/radio.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038FC91A-0C89-4E49-866C-75F0D1069E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="47">
   <si>
     <t>sexe</t>
   </si>
@@ -37,12 +38,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>hauteur de couverture radiculaire DM 1</t>
-  </si>
-  <si>
-    <t>HCRDM 2</t>
-  </si>
-  <si>
     <t>dent sur arcade</t>
   </si>
   <si>
@@ -155,13 +150,25 @@
   </si>
   <si>
     <t>mm</t>
+  </si>
+  <si>
+    <t>hcrdm_1</t>
+  </si>
+  <si>
+    <t>hcrdm_2</t>
+  </si>
+  <si>
+    <t>coverture_mesiale_preop</t>
+  </si>
+  <si>
+    <t>coverture_laterale_preop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +178,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -202,10 +217,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -482,41 +497,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AC1"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="34.85546875" customWidth="1"/>
-    <col min="7" max="7" width="36.42578125" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" customWidth="1"/>
-    <col min="13" max="13" width="34.42578125" customWidth="1"/>
-    <col min="14" max="14" width="33.7109375" customWidth="1"/>
-    <col min="15" max="15" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="34.88671875" customWidth="1"/>
+    <col min="7" max="7" width="36.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="9" width="21.5546875" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="25.88671875" customWidth="1"/>
+    <col min="13" max="13" width="34.44140625" customWidth="1"/>
+    <col min="14" max="14" width="33.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.88671875" customWidth="1"/>
     <col min="17" max="17" width="38" customWidth="1"/>
-    <col min="23" max="23" width="19.7109375" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" customWidth="1"/>
+    <col min="23" max="23" width="19.6640625" customWidth="1"/>
+    <col min="24" max="24" width="15.44140625" customWidth="1"/>
     <col min="25" max="25" width="15" customWidth="1"/>
-    <col min="26" max="26" width="12.5703125" customWidth="1"/>
-    <col min="28" max="28" width="27.85546875" customWidth="1"/>
-    <col min="29" max="29" width="21.5703125" customWidth="1"/>
+    <col min="26" max="26" width="12.5546875" customWidth="1"/>
+    <col min="28" max="28" width="27.88671875" customWidth="1"/>
+    <col min="29" max="29" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -531,79 +546,79 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -669,22 +684,22 @@
         <v>100</v>
       </c>
       <c r="Y2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -750,22 +765,22 @@
         <v>100</v>
       </c>
       <c r="Y3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -831,22 +846,22 @@
         <v>100</v>
       </c>
       <c r="Y4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -893,7 +908,7 @@
       <c r="R5">
         <v>9.1020000000000003</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="3">
         <v>9.2539999999999996</v>
       </c>
       <c r="T5">
@@ -912,22 +927,22 @@
         <v>100</v>
       </c>
       <c r="Y5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -993,27 +1008,27 @@
         <v>100</v>
       </c>
       <c r="Y6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2012</v>
@@ -1074,27 +1089,27 @@
         <v>100</v>
       </c>
       <c r="Y7" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>9</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
       </c>
       <c r="C8">
         <v>2018</v>
@@ -1155,27 +1170,27 @@
         <v>100</v>
       </c>
       <c r="Y8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>2017</v>
@@ -1236,22 +1251,22 @@
         <v>100</v>
       </c>
       <c r="Y9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1317,27 +1332,27 @@
         <v>75</v>
       </c>
       <c r="Y10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>2018</v>
@@ -1398,27 +1413,27 @@
         <v>100</v>
       </c>
       <c r="Y11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <v>2020</v>
@@ -1479,22 +1494,22 @@
         <v>75</v>
       </c>
       <c r="Y12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1560,22 +1575,22 @@
         <v>100</v>
       </c>
       <c r="Y13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1641,22 +1656,22 @@
         <v>100</v>
       </c>
       <c r="Y14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1722,22 +1737,22 @@
         <v>100</v>
       </c>
       <c r="Y15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1803,27 +1818,27 @@
         <v>100</v>
       </c>
       <c r="Y16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>2014</v>
@@ -1884,22 +1899,22 @@
         <v>100</v>
       </c>
       <c r="Y17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1965,22 +1980,22 @@
         <v>100</v>
       </c>
       <c r="Y18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2046,22 +2061,22 @@
         <v>75</v>
       </c>
       <c r="Y19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2127,22 +2142,22 @@
         <v>100</v>
       </c>
       <c r="Y20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2208,27 +2223,27 @@
         <v>100</v>
       </c>
       <c r="Y21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA21" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22">
         <v>2015</v>
@@ -2283,28 +2298,28 @@
         <v>2.1469999999999998</v>
       </c>
       <c r="W22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X22" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Y22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="Z22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AA22" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AB22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2370,22 +2385,22 @@
         <v>100</v>
       </c>
       <c r="Y23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AC23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2451,22 +2466,22 @@
         <v>100</v>
       </c>
       <c r="Y24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2532,22 +2547,22 @@
         <v>100</v>
       </c>
       <c r="Y25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2613,22 +2628,22 @@
         <v>100</v>
       </c>
       <c r="Y26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2694,198 +2709,198 @@
         <v>75</v>
       </c>
       <c r="Y27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Z27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AA27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AB27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="L29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="27.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="27.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B6" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18"/>
+      <c r="B18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>